<commit_message>
Processing in Chunk; Processing before user confirmation; status for each row added
</commit_message>
<xml_diff>
--- a/contacts/Contacts Template.xlsx
+++ b/contacts/Contacts Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Works\Web Scraping\WhatsAppSendMsg\contacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99BADED1-0C6C-49C8-8A0E-36EA76688E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FB61F2-7968-4B92-8E68-76F415F51E86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6B009050-5FC3-49A9-ACA5-58AB896CF9AD}"/>
+    <workbookView xWindow="4680" yWindow="3276" windowWidth="17280" windowHeight="8964" xr2:uid="{6B009050-5FC3-49A9-ACA5-58AB896CF9AD}"/>
   </bookViews>
   <sheets>
     <sheet name="any" sheetId="1" r:id="rId1"/>
@@ -25,15 +25,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>contact_number</t>
   </si>
   <si>
     <t>image_name</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>contact_name</t>
   </si>
 </sst>
 </file>
@@ -385,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6F90E9B-6D7C-45BF-A8B0-0ED2089082D7}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -397,14 +400,17 @@
     <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>